<commit_message>
Updated to run with xlrd
</commit_message>
<xml_diff>
--- a/PopData.xlsx
+++ b/PopData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="17256" windowHeight="5880"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="17256" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Aggregate Population Data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Year</t>
   </si>
@@ -39,13 +36,19 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Everywhere</t>
+  </si>
+  <si>
+    <t>Nothing at all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,15 +58,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,7 +88,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,7 +372,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,24 +383,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2500</v>
+      </c>
+      <c r="B2" s="2">
+        <v>90000000000</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>